<commit_message>
Update (again) TO FIX
</commit_message>
<xml_diff>
--- a/docs/Parte Escrita/Correções para versão final/TO FIX.xlsx
+++ b/docs/Parte Escrita/Correções para versão final/TO FIX.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>TO DO</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Juntar tudo no arquivo principal</t>
+  </si>
+  <si>
+    <t>objetivos, problema, justificativa e metodologia são subtopicos de introdução</t>
   </si>
 </sst>
 </file>
@@ -148,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -163,6 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{721703C5-34ED-410E-BA6C-3297B9CA7FC6}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,131 +542,138 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
+      <c r="A2" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3"/>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>9</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>5</v>
+      <c r="A15" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:B15">
+  <conditionalFormatting sqref="A3:B16 B2">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="&quot;&quot;">
       <formula>NOT(ISERROR(SEARCH("""""",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B15">
+  <conditionalFormatting sqref="B2:B16">
     <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:C15">
+  <conditionalFormatting sqref="B2:C16">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(B2))&gt;0</formula>
     </cfRule>

</xml_diff>